<commit_message>
dist y corrección sleeptime driver
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODE\WppBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D77E74E-3C78-4AAC-8A6D-945ADD27D2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC49AA7E-6C2F-4F68-9155-E916251FA605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3672" yWindow="480" windowWidth="15060" windowHeight="11652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="1" r:id="rId1"/>

</xml_diff>